<commit_message>
Work on ALU code to C# translation
</commit_message>
<xml_diff>
--- a/Y2021/Puzzle24/Puzzle24-Subprograms-x14.xlsx
+++ b/Y2021/Puzzle24/Puzzle24-Subprograms-x14.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\AdventOfCode\Y2021\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\AdventOfCode\Y2021\Puzzle24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C061C6-E19A-4E0C-BC70-761BEFE1A101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F65590-FE12-4EF8-9B71-BB37D5FE9780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="1665" windowWidth="23910" windowHeight="17145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs" sheetId="1" r:id="rId1"/>
-    <sheet name="Simplify to C#" sheetId="4" r:id="rId2"/>
-    <sheet name="Works" sheetId="3" r:id="rId3"/>
+    <sheet name="Simplify to C# 1" sheetId="5" r:id="rId2"/>
+    <sheet name="Simplify to C# Full" sheetId="4" r:id="rId3"/>
+    <sheet name="Works" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="75">
   <si>
     <t xml:space="preserve">inp w </t>
   </si>
@@ -231,6 +232,33 @@
   </si>
   <si>
     <t>Backward</t>
+  </si>
+  <si>
+    <t>NOP -OR- z /= 26;</t>
+  </si>
+  <si>
+    <t>x += B;</t>
+  </si>
+  <si>
+    <t>x = (x == w) ? 1 : 0</t>
+  </si>
+  <si>
+    <t>x = (x == 0) 1 ? 0;</t>
+  </si>
+  <si>
+    <t>y = 0 -OR- 25;</t>
+  </si>
+  <si>
+    <t>y = 1 -OR- 26;</t>
+  </si>
+  <si>
+    <t>z *= 1 -OR- 26;</t>
+  </si>
+  <si>
+    <t>y = 0 -OR- y;</t>
+  </si>
+  <si>
+    <t>z1 = z + y;</t>
   </si>
 </sst>
 </file>
@@ -388,7 +416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,6 +596,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -744,7 +778,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -789,6 +823,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="20" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2124,11 +2166,541 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB8CEEE-F0B0-4857-9C51-D2CDA5574AC5}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="4" style="1" customWidth="1"/>
+    <col min="9" max="9" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7">
+        <f>B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="7">
+        <f t="shared" ref="D1:F1" si="0">C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <f t="shared" ref="A4:A19" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890DBAC4-5DF0-434D-B1BC-14DF8B1572E1}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,7 +3213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Solve Puzzle 24 Part 2
</commit_message>
<xml_diff>
--- a/Y2021/Puzzle24/Puzzle24-Subprograms-x14.xlsx
+++ b/Y2021/Puzzle24/Puzzle24-Subprograms-x14.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\AdventOfCode\Y2021\Puzzle24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F65590-FE12-4EF8-9B71-BB37D5FE9780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFD5F41-DADE-41B0-B6FC-32D2A41924AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1665" windowWidth="23910" windowHeight="17145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="1665" windowWidth="23910" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs" sheetId="1" r:id="rId1"/>
     <sheet name="Simplify to C# 1" sheetId="5" r:id="rId2"/>
     <sheet name="Simplify to C# Full" sheetId="4" r:id="rId3"/>
-    <sheet name="Works" sheetId="3" r:id="rId4"/>
+    <sheet name="Final Stages Wksht" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="69">
   <si>
     <t xml:space="preserve">inp w </t>
   </si>
   <si>
-    <t>set x 0</t>
-  </si>
-  <si>
     <t>add x z</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>eql x 0</t>
   </si>
   <si>
-    <t>set y 0</t>
-  </si>
-  <si>
     <t>add y 25</t>
   </si>
   <si>
@@ -136,18 +130,6 @@
   </si>
   <si>
     <t>add z y</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>z</t>
   </si>
   <si>
     <t>div z 1</t>
@@ -265,6 +247,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -734,7 +720,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -777,8 +763,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -832,8 +819,12 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -861,6 +852,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1192,7 +1184,7 @@
   </sheetPr>
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1316,46 +1308,46 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="P3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="4"/>
     </row>
@@ -1365,46 +1357,46 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="4"/>
     </row>
@@ -1414,46 +1406,46 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="4"/>
     </row>
@@ -1463,52 +1455,52 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1517,52 +1509,52 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="N7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="P7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1571,46 +1563,46 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q8" s="4"/>
     </row>
@@ -1620,46 +1612,46 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
@@ -1669,46 +1661,46 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="N10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="O10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="P10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Q10" s="4"/>
     </row>
@@ -1718,46 +1710,46 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="P11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q11" s="4"/>
     </row>
@@ -1767,46 +1759,46 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q12" s="4"/>
     </row>
@@ -1816,46 +1808,46 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q13" s="4"/>
     </row>
@@ -1865,46 +1857,46 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q14" s="4"/>
     </row>
@@ -1914,46 +1906,46 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="N15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="O15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="P15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
@@ -1963,46 +1955,46 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q16" s="4"/>
     </row>
@@ -2012,52 +2004,52 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="H17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="J17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="N17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="O17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="P17" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2066,46 +2058,46 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q18" s="4"/>
     </row>
@@ -2115,46 +2107,46 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q19" s="4"/>
     </row>
@@ -2169,7 +2161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB8CEEE-F0B0-4857-9C51-D2CDA5574AC5}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -2227,7 +2219,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="9"/>
@@ -2238,19 +2230,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="10"/>
@@ -2262,19 +2254,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="10"/>
@@ -2286,22 +2278,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="9"/>
@@ -2312,25 +2304,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -2340,25 +2332,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>8</v>
-      </c>
       <c r="G7" s="20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -2368,22 +2360,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="9"/>
@@ -2394,22 +2386,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="9"/>
@@ -2420,19 +2412,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="10"/>
@@ -2444,22 +2436,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="9"/>
@@ -2470,22 +2462,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="9"/>
@@ -2496,22 +2488,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="9"/>
@@ -2522,22 +2514,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="9"/>
@@ -2548,19 +2540,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="10"/>
@@ -2572,22 +2564,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="9"/>
@@ -2598,25 +2590,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="G17" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I17" s="9"/>
     </row>
@@ -2626,22 +2618,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="9"/>
@@ -2652,40 +2644,40 @@
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="15"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2755,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H2" s="10"/>
     </row>
@@ -2765,22 +2757,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="H3" s="10"/>
     </row>
@@ -2790,22 +2782,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H4" s="10"/>
     </row>
@@ -2815,22 +2807,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H5" s="10"/>
     </row>
@@ -2840,25 +2832,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2867,25 +2859,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>8</v>
-      </c>
       <c r="G7" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2894,22 +2886,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H8" s="10"/>
     </row>
@@ -2919,22 +2911,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H9" s="10"/>
     </row>
@@ -2944,22 +2936,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H10" s="10"/>
     </row>
@@ -2969,22 +2961,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H11" s="10"/>
     </row>
@@ -2994,22 +2986,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H12" s="10"/>
     </row>
@@ -3019,22 +3011,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H13" s="10"/>
     </row>
@@ -3044,22 +3036,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H14" s="10"/>
     </row>
@@ -3069,22 +3061,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H15" s="10"/>
     </row>
@@ -3094,22 +3086,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H16" s="10"/>
     </row>
@@ -3119,25 +3111,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="G17" s="14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3146,22 +3138,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H18" s="10"/>
     </row>
@@ -3171,39 +3163,39 @@
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H19" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3214,313 +3206,588 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3B9526-F91E-4DA2-9657-D13D4997875C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="6" width="5.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="12" width="5.28515625" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="17" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7">
+        <v>10</v>
+      </c>
+      <c r="D1" s="7">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="7">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7">
+        <v>13</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <f t="shared" ref="A4:A19" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="S4" s="26"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="2">
+      <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="D7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="2">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="B19" s="25"/>
+      <c r="C19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M19" t="s">
-        <v>33</v>
-      </c>
+      <c r="D19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="77" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>